<commit_message>
Resolved Missing Lines Problem
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cobbk12org-my.sharepoint.com/personal/karen1_wright_cobbk12_org/Documents/Abdul/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{EC1866CB-E9AD-4BA1-A770-ED8115071111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8154666B-DFF5-4BF4-8CC8-84D619C249E9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{328DE7A9-A9F9-413E-809F-FA04DD8505BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{B3CE2467-DE4E-4E21-8981-75B9CEE0A554}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="231">
   <si>
     <t>Category</t>
   </si>
@@ -285,19 +285,450 @@
     <t>It would be extremely helpful for students to have a widget on their dashboard for "My Classes." This would decrease the number of clicks students need to use to navigate to a specific digital classroom, which is especially helpful for younger students and students with disabilities.</t>
   </si>
   <si>
-    <t>MAKE IT FASTER</t>
-  </si>
-  <si>
-    <t>In 2021-22, I could load up CTLS within 10 seconds. Worked flawlessly. It had few features, but it did what it needs to do - files and assignments.</t>
-  </si>
-  <si>
-    <t>Now, after this update, the loading speed is horrendous. CTLS fails to load 2 times out of 3, and even on a successful load it can take more than a minute. Clicks go unresponsive, it randomly times out. Ive cleared by cache &amp; tried multiple browsers. It doesn't happen with other websites.</t>
-  </si>
-  <si>
-    <t>Currently, CTLS is unusable. It is unacceptable that it takes 3-4 minutes for me to submit a SINGLE assignment when I used to be able to do it in 30 seconds.</t>
-  </si>
-  <si>
-    <t>My friends say the same things, so it's not an isolated issue. I am very technically savvy, and I have developed my own website and have set up an enterprise-grade network at my house, so I know a fair deal about networking. I know it's not my computer causing these slowdowns.</t>
+    <t>When building assessments in CTLS Assess, teachers need the ability to add sub-standards/learning targets to assessment items in addition to the standard. Subsequently, they need to be able to do reporting at the school level, teacher level, and individual student level based on how students performed on that sub-standard/learning target. This data needs to be evaluated using CTLS Reports as well as manipulated in Incite Analytics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This request supports the work that teachers do in their CCCs when doing grade-level and school wide interventions and is considered best practices. For example, if students were being assessed on ELAGSE6RL3, this standard could be broken down into several sub-standards/learning targets. Teachers would meet as a CCC and analyze the data based on how students performed on those individual sub-standards/learning targets and create intervention groups based on that data during their CCC meetings. They also would report this data on school-wide data sheets. So, the data needs to be seen in Reports as well as have the ability to be manipulated in Excel. </t>
+  </si>
+  <si>
+    <t>When building assessments in CTLS Assess, teachers need the ability to add sub-standards/learning targets to assessment items in addition to the standard. Subsequently, they need to be able to do reporting at the school level, teacher level, and individual student level based on how students performed on that sub-standard/learning target. This data needs to be evaluated using CTLS Reports as well as manipulated in Incite Analytics.
+This request supports the work that teachers do in their CCCs when doing grade-level and school wide interventions and is considered best practices. For example, if students were being assessed on ELAGSE6RL3, this standard could be broken down into several sub-standards/learning targets. Teachers would meet as a CCC and analyze the data based on how students performed on those individual sub-standards/learning targets and create intervention groups based on that data during their CCC meetings. They also would report this data on school-wide data sheets. So, the data needs to be seen in Reports as well as have the ability to be manipulated in Excel.</t>
+  </si>
+  <si>
+    <t>Thank You</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When building assessments in CTLS Assess, teachers need the ability to add sub-standards/learning targets to assessment items in addition to the standard. Subsequently, they need to be able to do reporting at the school level, teacher level, and individual student level based on how students performed on that sub-standard/learning target. This data needs to be evaluated using CTLS Reports as well as manipulated in Incite Analytics. </t>
+  </si>
+  <si>
+    <t>6. When building assessments in CTLS Assess, teachers need the ability to add sub-standards/learning targets to assessment items in addition to the standard. Subsequently, they need to be able to do reporting at the school level, teacher level, and individual student level based on how students performed on that sub-standard/learning target. This data needs to be evaluated using CTLS Reports as well as manipulated in Incite Analytics.
+7. This request supports the work that teachers do in their CCCs when doing grade-level and school wide interventions and is considered best practices. For example, if students were being assessed on ELAGSE6RL3, this standard could be broken down into several sub-standards/learning targets. Teachers would meet as a CCC and analyze the data based on how students performed on those individual sub-standards/learning targets and create intervention groups based on that data during their CCC meetings. They also would report this data on school-wide data sheets. So, the data needs to be seen in Reports as well as have the ability to be manipulated in Excel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. When building assessments in CTLS Assess, teachers need the ability to add sub-standards/learning targets to assessment items in addition to the standard. Subsequently, they need to be able to do reporting at the school level, teacher level, and individual student level based on how students performed on that sub-standard/learning target. This data needs to be evaluated using CTLS Reports as well as manipulated in Incite Analytics.      7. This request supports the work that teachers do in their CCCs when doing grade-level and school wide interventions and is considered best practices. For example, if students were being assessed on ELAGSE6RL3, this standard could be broken down into several sub-standards/learning targets. Teachers would meet as a CCC and analyze the data based on how students performed on those individual sub-standards/learning targets and create intervention groups based on that data during their CCC meetings. They also would report this data on school-wide data sheets. So, the data needs to be seen in Reports as well as have the ability to be manipulated in Excel.    </t>
+  </si>
+  <si>
+    <t>I'd like for there to be an option to gamify our modules by awarding badges and leaderboards using tasks completed in CTLS and not in CTLS (i.e. homework, class participation, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wanting to develop microlearning units where students can move at their own pace but make it fun. </t>
+  </si>
+  <si>
+    <t>Thank you</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please, change the settings in assignments. Students get a "green check" for opening an assignment NOT submitting it. When they go to review their classwork they think the green check means they submitted. Please change the settings so they ONLY get a green check if they do submit the assignment. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This often leads to unneccessary confusion. </t>
+  </si>
+  <si>
+    <t>My Digital Resources (students)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was using Headsprout on Clever via CTLS and now it is no longer accessible and saying that the license has expired. </t>
+  </si>
+  <si>
+    <t>It would be wonderful if it could be renewed or if more information would be shared about what to use in its place.</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Utilization Dashboard</t>
+  </si>
+  <si>
+    <t>I would like to see a way to send messages to students, I see the section to do so but students don't get these messages</t>
+  </si>
+  <si>
+    <t>This would be a great place for them to look for missing assignments or reminders that we send home via CTLS and give them the responsibility to keep up with their assignments since agendas have been taken out of the HS</t>
+  </si>
+  <si>
+    <t>I am now required to send OSS letters to parents via CTLS Messages. When I go to my home page (as shown in the PPT) I do not see any place for messages. I need to be able to send CTLS messages to parents. Thank you</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Assignments/discussion posts</t>
+  </si>
+  <si>
+    <t>Student assignments/discussion should be hidden until date they are assigned.</t>
+  </si>
+  <si>
+    <t>During the 2020 school year we had the ability to post an assignment for a future date and time. The assignment would not show up for the students until that date and time. Please bring this back. Students are attempting to complete preloaded assignments just because it shows up for them.</t>
+  </si>
+  <si>
+    <t>Please allow CCC teams to share drafts of posts. Our grade level teams share responsibilities. One of those is creating the newsletter. We have a school template for our newsletter. This does not transfer from word to CTLS posts well. If we could share draft of the newsletter written by one team mate on our school template, then share with the rest of the team, it would save a tremendous about of time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">share drafts of posts within CCC teams </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Always Available" option on Assignments needs to be moved to the bottom of the page with the other option buttons. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Always Available" and setting due date windows would be better placed with the other assignment option buttons like; "Allow Late Submission" at the bottom of the page. Grouping the assignment window with the parameters for submission and availability keeps it all in one place. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">add desmos to CTLS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">during testing, allowing students to get comfortable with the EOC calculator and practice what they will be assessed on. </t>
+  </si>
+  <si>
+    <t>Desmond calculator provided through CTLS assess is not the same Desmos calculator used on EOC. One issue in particular; the CTLS desk is calculator does not convert a decimal to a fraction (this action is provided on the desmos calculator used during EOC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is pertinent that this is fixed so my students are familiar with using the exact desmos calculator that they will use during EOC testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The scientific calculator in CTLS Assess does not mimic the calculator that Algebra students will have on the EOC. Is there any way that a feature can be added to mimic the Desmos Scientific Calculator? </t>
+  </si>
+  <si>
+    <t>This would be a wonderful feature to have for our students. Thank you!!</t>
+  </si>
+  <si>
+    <t>Enhancement Request: Visual Indicators for Published/Unpublished Coursework
+When copying coursework from one course to another, we often need to unpublish certain assignments. Currently, there is no way to easily identify unpublished items without clicking on each individual assignment, page, or booklet. It would be extremely helpful to have a visual indicator on the coursework homepage to distinguish between published and unpublished items. For example, using a different font color for unpublished items or adding a closed eye icon would save significant time.
+Please add the ability to select a unit when syncing to our Synergy gradebook. Currently, whenever assignments sync for the first time or with each update in CTLS, we have to manually reassign each assignment to the correct unit. This process needs to be repeated 3 or 4 times, which is inefficient and time-consuming.</t>
+  </si>
+  <si>
+    <t>Help streamline the workload.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please make it so teachers can see all of the student entries when a string input is received from the student users for a question. Currently, no report shows this. </t>
+  </si>
+  <si>
+    <t>This is a fundamental need for assessments.</t>
+  </si>
+  <si>
+    <t>Currently, when creating a post in CTLS Parent, teachers have the options to "Post Now," "Schedule," "Save Draft," and "Preview." However, when adding a new topic in the classboard, the only available options are "Cancel" and "Add Topic."
+I believe it would be highly beneficial to add a "Schedule" option for classboard topics. This feature would enable teachers to prepare their weekly class board updates in advance, such as on a Wednesday during their planning period, and schedule it to be posted automatically at a specified time, like Sunday night.
+I think this functionality could significantly enhance the user experience for teachers, allowing them more flexibility and efficiency in managing their class communications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank You </t>
+  </si>
+  <si>
+    <t>I believe it would be highly beneficial to add a "Schedule" option for classboard topics. This feature would enable teachers to prepare their weekly class board updates in advance, such as on a Wednesday during their planning period, and schedule it to be posted automatically at a specified time, like Sunday night.</t>
+  </si>
+  <si>
+    <t>I think this functionality could significantly enhance the user experience for teachers, allowing them more flexibility and efficiency in managing their class communications.</t>
+  </si>
+  <si>
+    <t>Ease of use has been the trend for CTLS...this would keep that trend going...</t>
+  </si>
+  <si>
+    <t>Currently, when creating a post in CTLS Parent, teachers have the options to "Post Now," "Schedule," "Save Draft," and "Preview." However, when adding a new topic in the classboard, the only available options are "Cancel" and "Add Topic."
+It would be highly beneficial to add a "Schedule" option for classboard topics. This feature would enable teachers to prepare their weekly class board updates in advance, such as on a Wednesday during their planning period, and schedule it to be posted automatically at a specified time.</t>
+  </si>
+  <si>
+    <t>Currently, when creating a post in CTLS Parent, teachers have the options to "Post Now," "Schedule," "Save Draft," and "Preview." However, when adding a new topic in the classboard, the only available options are "Cancel" and "Add Topic."
+I believe it would be highly beneficial to add a "Schedule" option for classboard topics. This feature would enable teachers to prepare their weekly class board updates in advance, such as on a Wednesday during their planning period, and schedule it to be posted automatically at a specified time, like Sunday night.
+I think this functionality could significantly enhance the user experience for teachers, allowing them more flexibility and efficiency in managing their class communications.
+I think this functionality could significantly enhance the user experience for teachers, allowing them more flexibility and efficiency in managing their class communications.</t>
+  </si>
+  <si>
+    <t>This would make my work life easier. Thank you for considering this awesome idea.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would it be possible to have a freeform option when placing hot spots on the Hot Spot: Drag and Drop? That would be SUPER helpful! </t>
+  </si>
+  <si>
+    <t>Thanks, Patrick!</t>
+  </si>
+  <si>
+    <t>Remove the locking when designing coursework in digital classrooms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is frustrating to have it lock on you as you move from one section to another and then have to unlock every time. It is not friendly to a user who is trying to quickly build a folder/section in coursework. </t>
+  </si>
+  <si>
+    <t>Please add a matching item type to Assess. Pretty, pretty please!</t>
+  </si>
+  <si>
+    <t>Thanks, Patrick! 😊</t>
+  </si>
+  <si>
+    <t>Can we please be alerted of messages, like last year, so that we know when we have a message from a parent. There have been several times when I have not received the notice through email.</t>
+  </si>
+  <si>
+    <t>Restore the message alert on the side</t>
+  </si>
+  <si>
+    <t>I would like for CTLS to open the first time the icon is tapped. As it is, we teachers have to open it, close it, and open it again.</t>
+  </si>
+  <si>
+    <t>It is time consuming to continue to have to open and close the app.</t>
+  </si>
+  <si>
+    <t>Scheduled send</t>
+  </si>
+  <si>
+    <t>Would love a way to schedule a message to a parent for later so that I don't forget to respond.</t>
+  </si>
+  <si>
+    <t>I'd like to be able to include certain punctuation marks, specifically apostrophes, in the titles of assignments. Typing "Washingtons Farewell Address" makes me cringe.</t>
+  </si>
+  <si>
+    <t>I know it's a small ask, but I know many English teachers who would be grateful.</t>
+  </si>
+  <si>
+    <t>"Please allow CCC teams to share drafts of posts. Our grade level teams share responsibilities. One of those is creating the newsletter. We have a school template for our newsletter. This does not transfer from word to CTLS posts well. If we could share draft of the newsletter written by one team mate on our school template, then share with the rest of the team, it would save a tremendous about of time."</t>
+  </si>
+  <si>
+    <t>CTLS parent communication</t>
+  </si>
+  <si>
+    <t>Please allow CCC teams to share drafts of posts. Our grade level teams share responsibilities. One of those is creating the newsletter. We have a school template for our newsletter. This does not transfer from word to CTLS posts well. If we could share draft of the newsletter written by one team mate on our school template, then share with the rest of the team, it would save a tremendous about of time."</t>
+  </si>
+  <si>
+    <t>when transferring it from Word into CTLS, it doesn’t transfer well. This has been slowing down our process</t>
+  </si>
+  <si>
+    <t>Please allow CCC teams to share drafts of posts. Our grade level teams share responsibilities. One of those is creating the newsletter. We have a school template for our newsletter. This does not transfer from word to CTLS posts well. If we could share draft of the newsletter written by one team mate on our school template, then share with the rest of the team, it would save a tremendous amount of time.</t>
+  </si>
+  <si>
+    <t>We send newsletters via CTLS Parent with the template feature every week.</t>
+  </si>
+  <si>
+    <t>"Please allow CCC teams to share drafts of posts. Our grade level teams share responsibilities. One of those is creating the newsletter. We have a school template for our newsletter. This does not transfer from word to CTLS posts well. If we could share draft of the newsletter written by one team mate on our school template, then share with the rest of the team, it would save a tremendous about of time.</t>
+  </si>
+  <si>
+    <t>share draft of post in CTLS</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>This would also be beneficial to students that are absent as well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication with parents is so very challenging on CTLS. Please make a more direct button to click that is not hidden to contact parents directly. </t>
+  </si>
+  <si>
+    <t>I appreciate any attention to this matter since we have been told we are expected to strictly stick to CTLS parent for communication.</t>
+  </si>
+  <si>
+    <t>In the quick scoring section of CTLS, it is not possible to add a "missing" (M) to a project. The only options are number grades. It would be very helpful if we could go through and mark students that are missing in a bulk format. It is very cumbersome to mark students missing in the grading center, because you have to go into each student individually. (I have 35 kids in one of my classes)  I also teach at Kennesaw State University and they use D2L bright space there are a lot of great functions that would be worth mimicking in CTLS. I would be happy to talk with you over phone or email about some ideas. Thank you!</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Please add a report option that will allow me to print out a copy of the assessment with student answers visible.  This would be very helpful for 1-1 remediation and correction of student understanding.  Thank you.</t>
+  </si>
+  <si>
+    <t>Needed to help students fix understanding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can we bookmark CTLS onto our web browser. It will not let me log in. </t>
+  </si>
+  <si>
+    <t>Could we login to our CTLS with a bookmark?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would be really helpful to be able to communicate with parents and students in one message. As a high school teacher, I like to make students a part of the conversation about missing grades and steps to remediate. Please consider an improvement to the messaging pathway that would allow for messages to be directed to both parent and student in the same CTLS Parent message. </t>
+  </si>
+  <si>
+    <t>Item analysis for multi-part questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When retrieving item analysis for multi-part question, I cannot see which part of the multi-part question was most missed or the student responses within that multi-part question. I need to be able to see the item analysis for each question within the multi-part question. </t>
+  </si>
+  <si>
+    <t>Item analysis for an assessment comparing multiple teachers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To make data analysis easier, it would be ideal to have an item analysis report that would include the results for all teachers at the school that completed the same assessment, just like we can compare student performance across teachers that give the same assessment. </t>
+  </si>
+  <si>
+    <t>1. Teachers need to have the ability to message students and CC: parents so we can communicate to students and reinforce independence skills
+2. CTLS Parent messages should reveal if a parent has received and/or opened the message so teachers can have documentation</t>
+  </si>
+  <si>
+    <t>It is important for teachers to contact students directly through CTLS Parent &amp; CC: parents for documentation purposes instead of contacting students via StudentVUE or Outlook.</t>
+  </si>
+  <si>
+    <t>District Coursework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We would like to see the standard added in the student math course book to help when planning and implementing the math standards. We would like assessments for the math standards. </t>
+  </si>
+  <si>
+    <t>Help please!</t>
+  </si>
+  <si>
+    <t>We would like to see the standards added in the student math coursebook to help when planning and implementing the second-grade math standards.
+We would also like common second-grade math assessments to be provided similar to other grade levels. This will help provide consistency throughout classes and schools in the district.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our team struggles to find consistency between the report card, district coursework, and the standards. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We would like to see the standard added in the student math course book to help when planning and implementing the 2nd grade math standards. We would also like common math assessments to be provided similar to what has been created for other grade levels. This will help provide consistency throughout classes and schools in the district. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our grade level team has struggled to find consistency between the report card, district coursework, and the standards. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We would like to see the standard added in the student math coursebook to help when planning and implementing the 2nd grade math standards.  In addition, we would also like common math assessments provided similar to other grade levels. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will help provide consistency throughout classes and schools in the district. Our team struggles to find consistency between the standards, district coursework, and district report card. rubric. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We would like to see the standards added in the student math coursebook to help when planning and implementing the 2nd grade math standards.  We would also like common math assessments to be provided similar to what has been created for other grade levels.  The will help provide consistency throughout classes and schools within the district.  </t>
+  </si>
+  <si>
+    <t>Our grade level has struggled to find consistency between the report card, district coursework, and the standards.</t>
+  </si>
+  <si>
+    <t>We would like to see the standards added to the student math workbook to help when planning and implementing the second grade math standards.
+We would also like common second grade math assessments to be provided similar to what has been created for other grade levels. This will help provide consistency throughout classes and schools in the district.</t>
+  </si>
+  <si>
+    <t>Our team struggles to find consistency among the report card, district coursework, and the standards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would be benefical to have the units and lessons labeled by quarter in math district coursework. </t>
+  </si>
+  <si>
+    <t>This would help with planning and instruction for teachers across the district.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We would like to see the standard added in the student math course book to help when planning and implementing the 2nd grade math standards.  the.  We would also like common math assessments to be provided similar to what other grade levels have been provided. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will help provide consistency throughout classes and schools throughout the district. Our team is having trouble with consistency between the report card, district coursework, and the standards. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We would like to see the standards added to the student math course book to help when planning and implementing the 2nd-grade math standards.  We would also like common math assessments to be provided similar to other grade levels.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please add the feature to be able to schedule Board Posts within a digital classroom.  Also, it would be helpful to be able to copy and paste working links into a board post.  </t>
+  </si>
+  <si>
+    <t>This enhancement is necessary to cut down on the time it takes to link and plan CTLS lessons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please add the feature to be able to schedule Board Posts within a digital classroom. Also, it would be helpful to copy and paste working links into a board post. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This enhancement is necessary to cut down on the time to link and plan CTLS lessons. </t>
+  </si>
+  <si>
+    <t>More digital resources for Kindergarten Math and ELA to be used by the students (e.g. Dreambox, Headsprout)</t>
+  </si>
+  <si>
+    <t>More resources for K students to use within CTLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am carrying over assignments from last year, but the only way for me to view them is to publish them again and then copy them over. I should be able to have access to all my materials published or unpublished. There should be a way for teachers to move materials with out the students being able to see it until I am ready for them to see it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This would just stream line the use of CTLS, </t>
+  </si>
+  <si>
+    <t>Unit 2 Outline does not show Multiplication, rather it shows Measurement and Data Reasoning.</t>
+  </si>
+  <si>
+    <t>If the Units could be matched up it would make for a more streamlined experience</t>
+  </si>
+  <si>
+    <t>Please add the ability to use the delete key in the typing session.</t>
+  </si>
+  <si>
+    <t>For some reason. we can use ctrl+delete, which deletes the entire word to the right of the input line, but not delete, which allows one to delete a single character instead.</t>
+  </si>
+  <si>
+    <t>I'd like to see an AI enhancement that would allow teachers to upload a premade question, from say on old test or a test prep book and have AI integrated so that it automatically select's the standards, depth of knowledge, revised blooms taxonomy, grade. content area language and tags. A lot of teachers use / create external tests as entering questions with all this information is too daunting. AI should be able to identify all that criteria and enter it automatically.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This would be an AI enhancement to CTLS Assess. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I would like to see CTLS Assess as a standalone app that locks out all browsers and tabs eliminating the chance of cheating. </t>
+  </si>
+  <si>
+    <t>CTLS Assess as a standalone App</t>
+  </si>
+  <si>
+    <t>Parents need access to previous year's report cards. Currently, if a parent doesn't download the report card from ParentVue they disappear when the new school year begins. This means the parent has to reach out to the school for copies of report cards. It would be great if yearend report cards were available in CTLS Parent assessment section for reference.</t>
+  </si>
+  <si>
+    <t>I very much need the ability to see all students answers to the questions at once. Please make it so that I can export a CSV file of responses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why? Because let's say a student miscalculates #5 then uses that mistake to calculate #6. If they correctly completed #6 but using their answer from #5, they are essentially punished twice for one mistake. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For individual student data (especially SPED and RTI students), it would be EXTREMELY helpful to be able to pull a report that includes the test questions and the individual student's answers. Special education teachers are constantly being asked to pull this information as evidence of progress toward meeting their individualized goals. </t>
+  </si>
+  <si>
+    <t>Having this as a report option would decrease special education teachers' workloads by hours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase the timeout limit before CTLS automatically logs out or allow teachers to set their own timeout limits. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am timing out of CTLS multiple times during each class and having to go through the process of re-logging in and it's killing precious class time. Either increase the timeout limit, or create a setting where teachers can set their own timeout limits. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would be cool if we had the option to export the grades of a specific assignment from the Grading Center into an Excel or something. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This can help teachers with gradebooks, data aggregation, and documentation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teachers have been asking for CTLS Parent sto allow them to assign time slots but then allow for RSVP. They like the RSVP feature but want to schedule the times for them. Currently, you can only add names after the  sign up is created and delivered to parents. </t>
+  </si>
+  <si>
+    <t>Ask from many teachers this year</t>
+  </si>
+  <si>
+    <t>Please allow teachers to DISABLE the automatic gradebook sync from Assess.</t>
+  </si>
+  <si>
+    <t>Some teachers input grades manually and would like to disable this feature.  Others would like to disable it once the majority of the class has taken the test, so that it doesn't create a new entry in the gradebook each time a student takes a make-up test.</t>
+  </si>
+  <si>
+    <t>There needs to be a report that shows the assessment questions and the students' answers. This would benefit both teachers who are analyzing the data and reviewing the responses, especially Special Education teachers who need individual student work samples.</t>
+  </si>
+  <si>
+    <t>add an option when creating an assignment on Student Coursework to be notified via email for assignments that are uploaded after the due date.</t>
+  </si>
+  <si>
+    <t>For some reason, students are not informing us (they think we already know?) when they are uploading assignments late if they were absent or just turning it in for the penalized grade.  It is not a reasonable use of time to constantly monitor CTLS for graded work on past assignments. An email option to let us know when something is uploaded after the date would help.</t>
+  </si>
+  <si>
+    <t>When using the lockdown feature on CTLS asses, students using an IPad can click outside of the assessment and see other sites.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there a way to enlarge the window when students are testing in CTLS ACCESS? It is difficult for me to view the active windows (heads up and data grid) when our students are testing. This makes scrolling difficult as well because the window is smaller, and we have to keep dragging our mouse. If there is a way to fix this on my end, please let me know. Thank you. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have had other teachers express their frustration with the viewing window when I asked them if they knew how to fix it. </t>
+  </si>
+  <si>
+    <t>Ability to upload more than one document at a time</t>
+  </si>
+  <si>
+    <t>When uploading documents in student coursework, I would like to upload multiple documents at a time. Right now, I have to choose one file at a time to upload. This is time consuming and tedious for five high school courses.</t>
+  </si>
+  <si>
+    <t>I would like for there to be a way to customize the student dashboard as I can the digital classroom. The widgets I move are only available on the student side after they find and click the small button for "Custom" which is very difficult for them to find. We are trying to bring "shortcuts" to the top for student ease of access.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>MAKE IT FASTER
+In 2021-22, I could load up CTLS within 10 seconds. Worked flawlessly. It had few features, but it did what it needs to do - files and assignments.
+Now, after this update, the loading speed is horrendous. CTLS fails to load 2 times out of 3, and even on a successful load it can take more than a minute. Clicks go unresponsive, it randomly times out. Ive cleared by cache &amp; tried multiple browsers. It doesn't happen with other websites.
+Currently, CTLS is unusable. It is unacceptable that it takes 3-4 minutes for me to submit a SINGLE assignment when I used to be able to do it in 30 seconds.
+My friends say the same things, so it's not an isolated issue. I am very technically savvy, and I have developed my own website and have set up an enterprise-grade network at my house, so I know a fair deal about networking. I know it's not my computer causing these slowdowns.</t>
   </si>
   <si>
     <t>Please make it so if you take a test on CTLS Assess, the grade automatically goes into Synergy.</t>
@@ -313,13 +744,25 @@
   </si>
   <si>
     <t xml:space="preserve">Make the instructions so easy to read and understand for parents </t>
+  </si>
+  <si>
+    <t>Recycle Bin for "Deleted" Entries in My Portfolio</t>
+  </si>
+  <si>
+    <t>In "My Portfolio", students can delete portfolio entries. However, if they accidentally delete something important, there is no way to get it back. It would be beneficial if there was a Recycle Bin or something of that sort. The "delete" button would be renamed to "Move to Trash" and it would move the file into the recycle bin. After some time period, maybe 30 days, the recycle bin would permanently delete the file. This would be beneficial since students can misunderstand things at times and may need this as a backup in case they accidentally delete something important.</t>
+  </si>
+  <si>
+    <t>Add Delete Button to files in the file explorer on the left panel</t>
+  </si>
+  <si>
+    <t>1. Please add an option to upload pictures since that might help you. 2. There is no delete button for files in the file explorer pane on the left hand side. There is a delete button for folders, however, adding a delete button for files would significantly improve efficiency.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,7 +793,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +809,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
         <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -406,7 +855,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -415,9 +864,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -429,9 +875,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -448,10 +903,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -751,20 +1202,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515B3478-0EDC-46EF-91BF-ACD27C3B5788}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="56.7109375" customWidth="1"/>
     <col min="3" max="3" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -775,423 +1226,1329 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:3" ht="30">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:3" ht="60">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" ht="60">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:3" ht="30">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="1:3" ht="90">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:3" ht="45">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:3" ht="60">
+      <c r="A8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:3" ht="90">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:3" ht="60">
+      <c r="A10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:3" ht="105">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:3" ht="120">
+      <c r="A12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:3" ht="90">
+      <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:3" ht="135">
+      <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="1:3" ht="45">
+      <c r="A15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:3" ht="60">
+      <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:3" ht="90">
+      <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="8" t="s">
+    <row r="18" spans="1:3" ht="45">
+      <c r="A18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:3" ht="90">
+      <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:3" ht="105">
+      <c r="A21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="1:3" ht="45">
+      <c r="A22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:3" ht="90">
+      <c r="A23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:3" ht="45">
+      <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="8" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="8" t="s">
+    <row r="26" spans="1:3" ht="60">
+      <c r="A26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="8" t="s">
+    <row r="27" spans="1:3" ht="150">
+      <c r="A27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="8" t="s">
+    <row r="28" spans="1:3" ht="60">
+      <c r="A28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="8" t="s">
+    <row r="29" spans="1:3" ht="45">
+      <c r="A29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="8" t="s">
+    <row r="30" spans="1:3" ht="90">
+      <c r="A30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="8" t="s">
+    <row r="31" spans="1:3" ht="30">
+      <c r="A31" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:3" ht="152.25">
+      <c r="A32" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="8" t="s">
+    <row r="33" spans="1:3" ht="30">
+      <c r="A33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="8" t="s">
+    <row r="34" spans="1:3" ht="135">
+      <c r="A34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="8" t="s">
+    <row r="35" spans="1:3" ht="30">
+      <c r="A35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:3" ht="105">
+      <c r="A37" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="8" t="s">
+    <row r="38" spans="1:3" ht="45">
+      <c r="A38" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+    <row r="39" spans="1:3" ht="75">
+      <c r="A39" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="40" spans="1:3" ht="183">
+      <c r="A40" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="290.25">
+      <c r="A41" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="183">
+      <c r="A42" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="183">
+      <c r="A43" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="290.25">
+      <c r="A44" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="45.75">
+      <c r="A45" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="290.25">
+      <c r="A46" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="76.5">
+      <c r="A47" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="30.75">
+      <c r="A48" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="290.25">
+      <c r="A49" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="60.75">
+      <c r="A50" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="60.75">
+      <c r="A51" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="76.5">
+      <c r="A52" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="106.5">
+      <c r="A53" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="76.5">
+      <c r="A54" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="30.75">
+      <c r="A55" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="76.5">
+      <c r="A56" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="60.75">
+      <c r="A57" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="244.5">
+      <c r="A58" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="45.75">
+      <c r="A59" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="183">
+      <c r="A60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="76.5">
+      <c r="A61" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="183">
+      <c r="A62" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="137.25">
+      <c r="A63" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="229.5">
+      <c r="A64" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="45.75">
+      <c r="A65" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="60.75">
+      <c r="A66" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="16.5">
+      <c r="A67" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="60.75">
+      <c r="A68" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="30.75">
+      <c r="A69" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30.75">
+      <c r="A70" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="45.75">
+      <c r="A71" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="106.5">
+      <c r="A72" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="106.5">
+      <c r="A73" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="106.5">
+      <c r="A74" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="106.5">
+      <c r="A75" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="106.5">
+      <c r="A76" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="106.5">
+      <c r="A77" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="106.5">
+      <c r="A78" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="106.5">
+      <c r="A79" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="106.5">
+      <c r="A80" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="229.5">
+      <c r="A81" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="106.5">
+      <c r="A82" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="183">
+      <c r="A83" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="45.75">
+      <c r="A84" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="167.25">
+      <c r="A85" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="60.75">
+      <c r="A86" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="30.75">
+      <c r="A87" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="106.5">
+      <c r="A88" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="76.5">
+      <c r="A89" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="76.5">
+      <c r="A90" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="91.5">
+      <c r="A91" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="45.75">
+      <c r="A92" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="91.5">
+      <c r="A93" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="91.5">
+      <c r="A94" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="60.75">
+      <c r="A95" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="91.5">
+      <c r="A96" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="106.5">
+      <c r="A97" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="30.75">
+      <c r="A98" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="76.5">
+      <c r="A99" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B99" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="60.75">
+      <c r="A100" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="45.75">
+      <c r="A101" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="45.75">
+      <c r="A102" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="30.75">
+      <c r="A103" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="91.5">
+      <c r="A104" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="30.75">
+      <c r="A105" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="45.75">
+      <c r="A106" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="121.5">
+      <c r="A107" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="30.75">
+      <c r="A108" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="91.5">
+      <c r="A109" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="60.75">
+      <c r="A110" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="91.5">
+      <c r="A111" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="76.5">
+      <c r="A112" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B112" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="45.75">
+      <c r="A113" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B113" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="76.5">
+      <c r="A114" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="76.5">
+      <c r="A115" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="76.5">
+      <c r="A116" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="106.5">
+      <c r="A117" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="30.75">
+      <c r="A118" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="91.5">
+      <c r="A119" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B119" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="60.75">
+      <c r="A120" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="91.5">
+      <c r="A121" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A39" xr:uid="{515B3478-0EDC-46EF-91BF-ACD27C3B5788}"/>
@@ -1202,154 +2559,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77765001-DB4E-49A4-9B76-06BC2231EBCA}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="46.140625" customWidth="1"/>
     <col min="2" max="2" width="79.140625" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="198">
+      <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>79</v>
+      <c r="B2" s="6" t="s">
+        <v>221</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="3" spans="1:6" ht="30.75">
+      <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B3" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B4" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45">
+      <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B5" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45">
+      <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>88</v>
+      <c r="B6" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="171.75" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="210.75" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="181.5" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60.75">
+      <c r="A10" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>